<commit_message>
Finalizado el valuador y el lector. Independizados los módulos.
</commit_message>
<xml_diff>
--- a/archivos/andina-mini-ACTUALIZADO.xlsx
+++ b/archivos/andina-mini-ACTUALIZADO.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,6 +452,11 @@
           <t>Nuevo Precio</t>
         </is>
       </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Última fecha</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -471,7 +476,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>DISTRIBUIDORA ANDINA</t>
+          <t>ANDINA</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -482,6 +487,11 @@
       <c r="F2" t="inlineStr">
         <is>
           <t>$ 764.40</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2023-12-29 00:00:00</t>
         </is>
       </c>
     </row>
@@ -503,13 +513,18 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>DISTRIBUIDORA ANDINA</t>
+          <t>ANDINA</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>$ 2610.00</t>
+          <t>Sin precio</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2023-12-29 00:00:00</t>
         </is>
       </c>
     </row>

</xml_diff>